<commit_message>
Added locked ring buffer implementation which works. Also added in timings so now all that needs doing is to add a lockless algorithm and test the two modes.
</commit_message>
<xml_diff>
--- a/Test_Data.xlsx
+++ b/Test_Data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Data Structure</t>
   </si>
@@ -30,22 +30,16 @@
     <t>Lockless</t>
   </si>
   <si>
-    <t>100 Iterations</t>
-  </si>
-  <si>
-    <t>1000 Iterations</t>
-  </si>
-  <si>
-    <t>10000 Iterations</t>
-  </si>
-  <si>
-    <t>100000 Iterations</t>
-  </si>
-  <si>
-    <t>1000000 Iterations</t>
-  </si>
-  <si>
     <t>All data measured in microseconds</t>
+  </si>
+  <si>
+    <t>Architecture</t>
+  </si>
+  <si>
+    <t>Iterations</t>
+  </si>
+  <si>
+    <t>64 Core Intel Xeon CPU E7-4820 @ 2.00GHz (Stoker)</t>
   </si>
 </sst>
 </file>
@@ -384,84 +378,94 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" customWidth="1"/>
-    <col min="3" max="7" width="17.28515625" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="32.42578125" customWidth="1"/>
+    <col min="2" max="2" width="46.42578125" customWidth="1"/>
+    <col min="4" max="8" width="17.28515625" customWidth="1"/>
+    <col min="9" max="9" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" t="s">
-        <v>8</v>
+      <c r="D2">
+        <v>100</v>
+      </c>
+      <c r="E2">
+        <v>1000</v>
+      </c>
+      <c r="F2">
+        <v>10000</v>
+      </c>
+      <c r="G2">
+        <v>100000</v>
+      </c>
+      <c r="H2">
+        <v>1000000</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
       <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
         <v>2</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>542</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>2960</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>12331</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>110053</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>1319244</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
         <v>3</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>522</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>1145</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>7264</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>69316</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>689642</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Tidied up the ring buffer code. I also collected some data from stoker and put it into excel with both locked and lockless modes. Next step is to collect data on my machine and add this to excel.
</commit_message>
<xml_diff>
--- a/Test_Data.xlsx
+++ b/Test_Data.xlsx
@@ -16,30 +16,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>Data Structure</t>
+    <t>64 Core Intel Xeon CPU E7-4820 @ 2.00GHz (Stoker) Locked</t>
   </si>
   <si>
-    <t>SPSC</t>
+    <t>64 Core Intel Xeon CPU E7-4820 @ 2.00GHz (Stoker) Lockless</t>
   </si>
   <si>
-    <t>Locked</t>
-  </si>
-  <si>
-    <t>Lockless</t>
-  </si>
-  <si>
-    <t>All data measured in microseconds</t>
-  </si>
-  <si>
-    <t>Architecture</t>
-  </si>
-  <si>
-    <t>Iterations</t>
-  </si>
-  <si>
-    <t>64 Core Intel Xeon CPU E7-4820 @ 2.00GHz (Stoker)</t>
+    <t>Ring Buffer</t>
   </si>
 </sst>
 </file>
@@ -75,8 +60,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -89,6 +77,352 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-IE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-IE"/>
+              <a:t>Ring Buffer</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>64 Core Intel Xeon CPU E7-4820 @ 2.00GHz (Stoker) Locked</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$C$10:$J$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$11:$J$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>4239367</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11258639</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11367927</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11446883</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13613810</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14013680</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14401700</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16928362</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>64 Core Intel Xeon CPU E7-4820 @ 2.00GHz (Stoker) Lockless</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$C$10:$J$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$12:$J$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>6694544</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14023982</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17133277</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17741859</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17947704</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18025342</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>18087549</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>18128032</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="99098624"/>
+        <c:axId val="99100544"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="99098624"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-IE"/>
+                  <a:t>Threads</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="99100544"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="99100544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Iterations</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> per second</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="99098624"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1009650</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>133349</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>971550</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>128586</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -378,10 +712,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
+  <dimension ref="B9:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B9" sqref="B9:J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -392,85 +726,110 @@
     <col min="9" max="9" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
+      <c r="F10">
+        <v>8</v>
+      </c>
+      <c r="G10">
+        <v>16</v>
+      </c>
+      <c r="H10">
+        <v>32</v>
+      </c>
+      <c r="I10">
+        <v>64</v>
+      </c>
+      <c r="J10">
+        <v>128</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
         <v>0</v>
       </c>
-      <c r="D2">
-        <v>100</v>
-      </c>
-      <c r="E2">
-        <v>1000</v>
-      </c>
-      <c r="F2">
-        <v>10000</v>
-      </c>
-      <c r="G2">
-        <v>100000</v>
-      </c>
-      <c r="H2">
-        <v>1000000</v>
+      <c r="C11">
+        <v>4239367</v>
+      </c>
+      <c r="D11">
+        <v>11258639</v>
+      </c>
+      <c r="E11">
+        <v>11367927</v>
+      </c>
+      <c r="F11">
+        <v>11446883</v>
+      </c>
+      <c r="G11">
+        <v>13613810</v>
+      </c>
+      <c r="H11">
+        <v>14013680</v>
+      </c>
+      <c r="I11">
+        <v>14401700</v>
+      </c>
+      <c r="J11">
+        <v>16928362</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
         <v>1</v>
       </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4">
-        <v>542</v>
-      </c>
-      <c r="E4">
-        <v>2960</v>
-      </c>
-      <c r="F4">
-        <v>12331</v>
-      </c>
-      <c r="G4">
-        <v>110053</v>
-      </c>
-      <c r="H4">
-        <v>1319244</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5">
-        <v>522</v>
-      </c>
-      <c r="E5">
-        <v>1145</v>
-      </c>
-      <c r="F5">
-        <v>7264</v>
-      </c>
-      <c r="G5">
-        <v>69316</v>
-      </c>
-      <c r="H5">
-        <v>689642</v>
+      <c r="C12">
+        <v>6694544</v>
+      </c>
+      <c r="D12">
+        <v>14023982</v>
+      </c>
+      <c r="E12">
+        <v>17133277</v>
+      </c>
+      <c r="F12">
+        <v>17741859</v>
+      </c>
+      <c r="G12">
+        <v>17947704</v>
+      </c>
+      <c r="H12">
+        <v>18025342</v>
+      </c>
+      <c r="I12">
+        <v>18087549</v>
+      </c>
+      <c r="J12">
+        <v>18128032</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B9:J9"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Gathered data from local machine, ducss and netsoc. VPN only has one core so I cannot use it. I tested the assembly spinlock against the c++ variant, minimal difference, hence I removed the assembly code from ring.cpp. Started adding to my report in a meaningful fashion.
</commit_message>
<xml_diff>
--- a/Test_Data.xlsx
+++ b/Test_Data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>64 Core Intel Xeon CPU E7-4820 @ 2.00GHz (Stoker) Locked</t>
   </si>
@@ -27,25 +27,28 @@
     <t>64 Core Intel Xeon CPU E7-4820 @ 2.00GHz (Stoker) C++ Spinlock</t>
   </si>
   <si>
-    <t>Ring Buffer - Size = Doesn't matter since addition/removal is only done at the top of the queue</t>
-  </si>
-  <si>
-    <t>4 Core Intel Core i5-2500K CPU @ 3.30GHz Locked</t>
-  </si>
-  <si>
-    <t>4 Core Intel Core i5-2500K CPU @ 3.30GHz C++ Spinlock</t>
-  </si>
-  <si>
-    <t>2 Core Intel Xeon CPU @ 3.00 GHz Locked</t>
-  </si>
-  <si>
-    <t>2 Core Intel Xeon CPU @ 3.00 GHz Spinlock</t>
-  </si>
-  <si>
-    <t>2 Core Intel Xeon CPU @ 2.80 GHz Locked</t>
-  </si>
-  <si>
-    <t>2 Core Intel Xeon CPU @ 2.80 GHz Spinlock</t>
+    <t>5328217 ,418741 ,473308 ,461109 ,448229 ,448645 ,436339 ,432057</t>
+  </si>
+  <si>
+    <t>2 Core Intel Xeon CPU @ 3.00 GHz Locked (Ducss)</t>
+  </si>
+  <si>
+    <t>2 Core Intel Xeon CPU @ 2.80 GHz Locked (Netsoc)</t>
+  </si>
+  <si>
+    <t>4 Core Intel Core i5-2500K CPU @ 3.30GHz (Local) Locked</t>
+  </si>
+  <si>
+    <t>4 Core Intel Core i5-2500K CPU @ 3.30GHz (Local) C++ Spinlock</t>
+  </si>
+  <si>
+    <t>2 Core Intel Xeon CPU @ 3.00 GHz Spinlock (Ducss)</t>
+  </si>
+  <si>
+    <t>2 Core Intel Xeon CPU @ 2.80 GHz Spinlock (Ducss)</t>
+  </si>
+  <si>
+    <t>Ring Buffer - Size (1000)= Doesn't matter since addition/removal is only done at the top of the queue</t>
   </si>
 </sst>
 </file>
@@ -387,10 +390,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A9:I18"/>
+  <dimension ref="A5:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:I18"/>
+      <selection activeCell="A10" sqref="A10:I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -400,9 +403,40 @@
     <col min="8" max="8" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>5328217</v>
+      </c>
+      <c r="C6">
+        <v>418741</v>
+      </c>
+      <c r="D6">
+        <v>473308</v>
+      </c>
+      <c r="E6">
+        <v>461109</v>
+      </c>
+      <c r="F6">
+        <v>448229</v>
+      </c>
+      <c r="G6">
+        <v>448645</v>
+      </c>
+      <c r="H6">
+        <v>436339</v>
+      </c>
+      <c r="I6">
+        <v>432057</v>
+      </c>
+    </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -499,32 +533,176 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="B13">
+        <v>5328217</v>
+      </c>
+      <c r="C13">
+        <v>418741</v>
+      </c>
+      <c r="D13">
+        <v>473308</v>
+      </c>
+      <c r="E13">
+        <v>461109</v>
+      </c>
+      <c r="F13">
+        <v>448229</v>
+      </c>
+      <c r="G13">
+        <v>448645</v>
+      </c>
+      <c r="H13">
+        <v>436339</v>
+      </c>
+      <c r="I13">
+        <v>432057</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="B14">
+        <v>10604337</v>
+      </c>
+      <c r="C14">
+        <v>10611323</v>
+      </c>
+      <c r="D14">
+        <v>10564897</v>
+      </c>
+      <c r="E14">
+        <v>10540146</v>
+      </c>
+      <c r="F14">
+        <v>10570471</v>
+      </c>
+      <c r="G14">
+        <v>10592364</v>
+      </c>
+      <c r="H14">
+        <v>10539685</v>
+      </c>
+      <c r="I14">
+        <v>10488351</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="B15">
+        <v>1321542</v>
+      </c>
+      <c r="C15">
+        <v>1495327</v>
+      </c>
+      <c r="D15">
+        <v>1467956</v>
+      </c>
+      <c r="E15">
+        <v>1254631</v>
+      </c>
+      <c r="F15">
+        <v>1363862</v>
+      </c>
+      <c r="G15">
+        <v>1767556</v>
+      </c>
+      <c r="H15">
+        <v>1358405</v>
+      </c>
+      <c r="I15">
+        <v>1373794</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="B16">
+        <v>1191029</v>
+      </c>
+      <c r="C16">
+        <v>1180264</v>
+      </c>
+      <c r="D16">
+        <v>1123372</v>
+      </c>
+      <c r="E16">
+        <v>1189681</v>
+      </c>
+      <c r="F16">
+        <v>1200067</v>
+      </c>
+      <c r="G16">
+        <v>1228259</v>
+      </c>
+      <c r="H16">
+        <v>1205112</v>
+      </c>
+      <c r="I16">
+        <v>1179244</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="B17">
+        <v>3421422</v>
+      </c>
+      <c r="C17">
+        <v>4856188</v>
+      </c>
+      <c r="D17">
+        <v>4855373</v>
+      </c>
+      <c r="E17">
+        <v>4557720</v>
+      </c>
+      <c r="F17">
+        <v>4723686</v>
+      </c>
+      <c r="G17">
+        <v>3093845</v>
+      </c>
+      <c r="H17">
+        <v>3169190</v>
+      </c>
+      <c r="I17">
+        <v>2640398</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>8</v>
+      </c>
+      <c r="B18">
+        <v>2560144</v>
+      </c>
+      <c r="C18">
+        <v>3529022</v>
+      </c>
+      <c r="D18">
+        <v>2567171</v>
+      </c>
+      <c r="E18">
+        <v>2586400</v>
+      </c>
+      <c r="F18">
+        <v>2599223</v>
+      </c>
+      <c r="G18">
+        <v>2575840</v>
+      </c>
+      <c r="H18">
+        <v>2522506</v>
+      </c>
+      <c r="I18">
+        <v>2445529</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added some references to the report, along with some more content
</commit_message>
<xml_diff>
--- a/Test_Data.xlsx
+++ b/Test_Data.xlsx
@@ -21,34 +21,34 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
-    <t>64 Core Intel Xeon CPU E7-4820 @ 2.00GHz (Stoker) Locked</t>
-  </si>
-  <si>
-    <t>64 Core Intel Xeon CPU E7-4820 @ 2.00GHz (Stoker) C++ Spinlock</t>
-  </si>
-  <si>
     <t>5328217 ,418741 ,473308 ,461109 ,448229 ,448645 ,436339 ,432057</t>
   </si>
   <si>
-    <t>2 Core Intel Xeon CPU @ 3.00 GHz Locked (Ducss)</t>
+    <t>Ring Buffer - Size (1000)= Doesn't matter since addition/removal is only done at the top of the queue</t>
   </si>
   <si>
-    <t>2 Core Intel Xeon CPU @ 2.80 GHz Locked (Netsoc)</t>
+    <t>64 Core Intel Xeon CPU E7-4820 @ 2.00GHz (A) Locked</t>
   </si>
   <si>
-    <t>4 Core Intel Core i5-2500K CPU @ 3.30GHz (Local) Locked</t>
+    <t>64 Core Intel Xeon CPU E7-4820 @ 2.00GHz (A) C++ Spinlock</t>
   </si>
   <si>
-    <t>4 Core Intel Core i5-2500K CPU @ 3.30GHz (Local) C++ Spinlock</t>
+    <t>4 Core Intel Core i5-2500K CPU @ 3.30GHz (B) Locked</t>
   </si>
   <si>
-    <t>2 Core Intel Xeon CPU @ 3.00 GHz Spinlock (Ducss)</t>
+    <t>4 Core Intel Core i5-2500K CPU @ 3.30GHz (B) C++ Spinlock</t>
   </si>
   <si>
-    <t>2 Core Intel Xeon CPU @ 2.80 GHz Spinlock (Ducss)</t>
+    <t>2 Core Intel CPU @ 3.00 GHz (C) Locked</t>
   </si>
   <si>
-    <t>Ring Buffer - Size (1000)= Doesn't matter since addition/removal is only done at the top of the queue</t>
+    <t>2 Core Intel CPU @ 3.00 GHz (C) Spinlock</t>
+  </si>
+  <si>
+    <t>2 Core Intel CPU @ 2.80 GHz (D) Locked</t>
+  </si>
+  <si>
+    <t>2 Core Intel CPU @ 2.80 GHz (D) Spinlock</t>
   </si>
 </sst>
 </file>
@@ -101,6 +101,782 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-IE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>64 Core Intel Xeon CPU E7-4820 @ 2.00GHz (A) Locked</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$10:$I$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$11:$I$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>6558774</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8914003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8757513</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8415938</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7775145</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4334278</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3166165</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3166369</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>64 Core Intel Xeon CPU E7-4820 @ 2.00GHz (A) C++ Spinlock</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$10:$I$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$12:$I$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>4235748</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7986304</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7533212</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4266191</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4239697</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4910270</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4221463</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3673234</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4 Core Intel Core i5-2500K CPU @ 3.30GHz (B) Locked</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$10:$I$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$13:$I$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>5328217</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>418741</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>473308</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>461109</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>448229</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>448645</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>436339</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>432057</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4 Core Intel Core i5-2500K CPU @ 3.30GHz (B) C++ Spinlock</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$10:$I$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$14:$I$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>10604337</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10611323</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10564897</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10540146</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10570471</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10592364</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10539685</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10488351</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2 Core Intel CPU @ 3.00 GHz (C) Locked</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$10:$I$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$15:$I$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1321542</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1495327</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1467956</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1254631</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1363862</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1767556</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1358405</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1373794</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2 Core Intel CPU @ 3.00 GHz (C) Spinlock</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$10:$I$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$16:$I$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1191029</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1180264</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1123372</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1189681</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1200067</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1228259</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1205112</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1179244</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$17</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2 Core Intel CPU @ 2.80 GHz (D) Locked</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$10:$I$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$17:$I$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>3421422</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4856188</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4855373</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4557720</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4723686</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3093845</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3169190</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2640398</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2 Core Intel CPU @ 2.80 GHz (D) Spinlock</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$10:$I$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$18:$I$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2560144</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3529022</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2567171</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2586400</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2599223</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2575840</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2522506</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2445529</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="53897088"/>
+        <c:axId val="53898624"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="53897088"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="53898624"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="53898624"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="53897088"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -393,7 +1169,7 @@
   <dimension ref="A5:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:I18"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -405,7 +1181,7 @@
   <sheetData>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -436,7 +1212,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -475,7 +1251,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B11">
         <v>6558774</v>
@@ -504,7 +1280,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B12">
         <v>4235748</v>
@@ -533,7 +1309,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B13">
         <v>5328217</v>
@@ -562,7 +1338,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B14">
         <v>10604337</v>
@@ -591,7 +1367,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B15">
         <v>1321542</v>
@@ -649,7 +1425,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B17">
         <v>3421422</v>
@@ -678,7 +1454,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B18">
         <v>2560144</v>
@@ -711,6 +1487,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added a TAS and ticket lock to all four machines and collected data from all of them.
</commit_message>
<xml_diff>
--- a/Test_Data.xlsx
+++ b/Test_Data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Ring Buffer - Size (1000)= Doesn't matter since addition/removal is only done at the top of the queue</t>
   </si>
@@ -27,36 +27,18 @@
     <t>64 Core Intel Xeon CPU E7-4820 @ 2.00GHz (A) Locked</t>
   </si>
   <si>
-    <t>64 Core Intel Xeon CPU E7-4820 @ 2.00GHz (A) C++ Spinlock</t>
-  </si>
-  <si>
     <t>4 Core Intel Core i5-2500K CPU @ 3.30GHz (B) Locked</t>
   </si>
   <si>
-    <t>4 Core Intel Core i5-2500K CPU @ 3.30GHz (B) C++ Spinlock</t>
-  </si>
-  <si>
-    <t>2 Core Intel CPU @ 3.00 GHz (C) Spinlock</t>
-  </si>
-  <si>
     <t>2 Core Intel CPU @ 2.80 GHz (D) Locked</t>
   </si>
   <si>
-    <t>2 Core Intel CPU @ 2.80 GHz (D) Spinlock</t>
-  </si>
-  <si>
     <t>64 Core Intel Xeon CPU E7-4820 @ 2.00GHz (A) CAS lock</t>
   </si>
   <si>
     <t>4 Core Intel Core i5-2500K CPU @ 3.30GHz (B) CAS lock</t>
   </si>
   <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
     <t>2 Core Intel CPU @ 3.00 GHz (C - Ducss) Locked</t>
   </si>
   <si>
@@ -64,6 +46,42 @@
   </si>
   <si>
     <t>2 Core Intel CPU @ 2.80 GHz (D) CAS lock</t>
+  </si>
+  <si>
+    <t>64 Core Intel Xeon CPU E7-4820 @ 2.00GHz (A) TTAS</t>
+  </si>
+  <si>
+    <t>4 Core Intel Core i5-2500K CPU @ 3.30GHz (B) TTAS</t>
+  </si>
+  <si>
+    <t>2 Core Intel CPU @ 3.00 GHz (C)  TTAS</t>
+  </si>
+  <si>
+    <t>2 Core Intel CPU @ 2.80 GHz (D) TTAS</t>
+  </si>
+  <si>
+    <t>64 Core Intel Xeon CPU E7-4820 @ 2.00GHz (A) TAS</t>
+  </si>
+  <si>
+    <t>4 Core Intel Core i5-2500K CPU @ 3.30GHz (B) TAS</t>
+  </si>
+  <si>
+    <t>2 Core Intel CPU @ 3.00 GHz (C)  TAS</t>
+  </si>
+  <si>
+    <t>2 Core Intel CPU @ 2.80 GHz (D) TAS</t>
+  </si>
+  <si>
+    <t>4 Core Intel Core i5-2500K CPU @ 3.30GHz (B) Ticket</t>
+  </si>
+  <si>
+    <t>64 Core Intel Xeon CPU E7-4820 @ 2.00GHz (A) Ticket</t>
+  </si>
+  <si>
+    <t>2 Core Intel CPU @ 3.00 GHz (C)  Ticket</t>
+  </si>
+  <si>
+    <t>2 Core Intel CPU @ 2.80 GHz (D) Ticket</t>
   </si>
 </sst>
 </file>
@@ -405,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A5:I22"/>
+  <dimension ref="A5:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -420,86 +438,28 @@
   <sheetData>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5">
-        <v>1</v>
+        <v>14077775</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>1075</v>
       </c>
       <c r="D5">
-        <v>4</v>
+        <v>2518</v>
       </c>
       <c r="E5">
-        <v>8</v>
+        <v>2235</v>
       </c>
       <c r="F5">
-        <v>16</v>
+        <v>2014</v>
       </c>
       <c r="G5">
-        <v>32</v>
+        <v>1364</v>
       </c>
       <c r="H5">
-        <v>64</v>
+        <v>1986</v>
       </c>
       <c r="I5">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6">
-        <v>5642544</v>
-      </c>
-      <c r="C6">
-        <v>8288701</v>
-      </c>
-      <c r="D6">
-        <v>5707577</v>
-      </c>
-      <c r="E6">
-        <v>5710434</v>
-      </c>
-      <c r="F6">
-        <v>7054031</v>
-      </c>
-      <c r="G6">
-        <v>5687563</v>
-      </c>
-      <c r="H6">
-        <v>7064434</v>
-      </c>
-      <c r="I6">
-        <v>5705941</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7">
-        <v>4995144</v>
-      </c>
-      <c r="C7">
-        <v>8292455</v>
-      </c>
-      <c r="D7">
-        <v>4981362</v>
-      </c>
-      <c r="E7">
-        <v>4983926</v>
-      </c>
-      <c r="F7">
-        <v>4987386</v>
-      </c>
-      <c r="G7">
-        <v>4990385</v>
-      </c>
-      <c r="H7">
-        <v>4995865</v>
-      </c>
-      <c r="I7">
-        <v>5005510</v>
+        <v>2618</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -572,7 +532,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B12">
         <v>5642544</v>
@@ -601,60 +561,60 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="B13">
-        <v>4235748</v>
+        <v>6163242</v>
       </c>
       <c r="C13">
-        <v>7986304</v>
+        <v>40341</v>
       </c>
       <c r="D13">
-        <v>7533212</v>
+        <v>15</v>
       </c>
       <c r="E13">
-        <v>4266191</v>
+        <v>29876</v>
       </c>
       <c r="F13">
-        <v>4239697</v>
+        <v>125211</v>
       </c>
       <c r="G13">
-        <v>4910270</v>
+        <v>39334</v>
       </c>
       <c r="H13">
-        <v>4221463</v>
+        <v>11527</v>
       </c>
       <c r="I13">
-        <v>3673234</v>
+        <v>39827</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B14">
-        <v>5328217</v>
+        <v>4910844</v>
       </c>
       <c r="C14">
-        <v>418741</v>
+        <v>5505544</v>
       </c>
       <c r="D14">
-        <v>473308</v>
+        <v>2979812</v>
       </c>
       <c r="E14">
-        <v>461109</v>
+        <v>715369</v>
       </c>
       <c r="F14">
-        <v>448229</v>
+        <v>215518</v>
       </c>
       <c r="G14">
-        <v>448645</v>
+        <v>130338</v>
       </c>
       <c r="H14">
-        <v>436339</v>
+        <v>66332</v>
       </c>
       <c r="I14">
-        <v>432057</v>
+        <v>36518</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -662,202 +622,202 @@
         <v>9</v>
       </c>
       <c r="B15">
-        <v>9771618</v>
+        <v>4235748</v>
       </c>
       <c r="C15">
-        <v>9735489</v>
+        <v>7986304</v>
       </c>
       <c r="D15">
-        <v>9905043</v>
+        <v>7533212</v>
       </c>
       <c r="E15">
-        <v>9916571</v>
+        <v>4266191</v>
       </c>
       <c r="F15">
-        <v>9639092</v>
+        <v>4239697</v>
       </c>
       <c r="G15">
-        <v>9802904</v>
+        <v>4910270</v>
       </c>
       <c r="H15">
-        <v>9930743</v>
+        <v>4221463</v>
       </c>
       <c r="I15">
-        <v>9515278</v>
+        <v>3673234</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B16">
-        <v>10604337</v>
+        <v>5328217</v>
       </c>
       <c r="C16">
-        <v>10611323</v>
+        <v>418741</v>
       </c>
       <c r="D16">
-        <v>10564897</v>
+        <v>473308</v>
       </c>
       <c r="E16">
-        <v>10540146</v>
+        <v>461109</v>
       </c>
       <c r="F16">
-        <v>10570471</v>
+        <v>448229</v>
       </c>
       <c r="G16">
-        <v>10592364</v>
+        <v>448645</v>
       </c>
       <c r="H16">
-        <v>10539685</v>
+        <v>436339</v>
       </c>
       <c r="I16">
-        <v>10488351</v>
+        <v>432057</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B17">
-        <v>1321542</v>
+        <v>9771618</v>
       </c>
       <c r="C17">
-        <v>1495327</v>
+        <v>9735489</v>
       </c>
       <c r="D17">
-        <v>1467956</v>
+        <v>9905043</v>
       </c>
       <c r="E17">
-        <v>1254631</v>
+        <v>9916571</v>
       </c>
       <c r="F17">
-        <v>1363862</v>
+        <v>9639092</v>
       </c>
       <c r="G17">
-        <v>1767556</v>
+        <v>9802904</v>
       </c>
       <c r="H17">
-        <v>1358405</v>
+        <v>9930743</v>
       </c>
       <c r="I17">
-        <v>1373794</v>
+        <v>9515278</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B18">
-        <v>1249352</v>
+        <v>14077775</v>
       </c>
       <c r="C18">
-        <v>1258630</v>
+        <v>1075</v>
       </c>
       <c r="D18">
-        <v>1438296</v>
+        <v>2518</v>
       </c>
       <c r="E18">
-        <v>1247512</v>
+        <v>2235</v>
       </c>
       <c r="F18">
-        <v>1438910</v>
+        <v>2014</v>
       </c>
       <c r="G18">
-        <v>1230792</v>
+        <v>1364</v>
       </c>
       <c r="H18">
-        <v>1438801</v>
+        <v>1986</v>
       </c>
       <c r="I18">
-        <v>1233541</v>
+        <v>2618</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B19">
-        <v>1191029</v>
+        <v>10644755</v>
       </c>
       <c r="C19">
-        <v>1180264</v>
+        <v>8292727</v>
       </c>
       <c r="D19">
-        <v>1123372</v>
+        <v>4840726</v>
       </c>
       <c r="E19">
-        <v>1189681</v>
+        <v>4499906</v>
       </c>
       <c r="F19">
-        <v>1200067</v>
+        <v>4600061</v>
       </c>
       <c r="G19">
-        <v>1228259</v>
+        <v>4661298</v>
       </c>
       <c r="H19">
-        <v>1205112</v>
+        <v>4934930</v>
       </c>
       <c r="I19">
-        <v>1179244</v>
+        <v>4789439</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B20">
-        <v>3421422</v>
+        <v>10604337</v>
       </c>
       <c r="C20">
-        <v>4856188</v>
+        <v>10611323</v>
       </c>
       <c r="D20">
-        <v>4855373</v>
+        <v>10564897</v>
       </c>
       <c r="E20">
-        <v>4557720</v>
+        <v>10540146</v>
       </c>
       <c r="F20">
-        <v>4723686</v>
+        <v>10570471</v>
       </c>
       <c r="G20">
-        <v>3093845</v>
+        <v>10592364</v>
       </c>
       <c r="H20">
-        <v>3169190</v>
+        <v>10539685</v>
       </c>
       <c r="I20">
-        <v>2640398</v>
+        <v>10488351</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B21">
-        <v>2642745</v>
+        <v>1321542</v>
       </c>
       <c r="C21">
-        <v>2716931</v>
+        <v>1495327</v>
       </c>
       <c r="D21">
-        <v>3473391</v>
+        <v>1467956</v>
       </c>
       <c r="E21">
-        <v>2658225</v>
+        <v>1254631</v>
       </c>
       <c r="F21">
-        <v>2654354</v>
+        <v>1363862</v>
       </c>
       <c r="G21">
-        <v>3450999</v>
+        <v>1767556</v>
       </c>
       <c r="H21">
-        <v>2577043</v>
+        <v>1358405</v>
       </c>
       <c r="I21">
-        <v>2596864</v>
+        <v>1373794</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -865,27 +825,259 @@
         <v>7</v>
       </c>
       <c r="B22">
+        <v>1249352</v>
+      </c>
+      <c r="C22">
+        <v>1258630</v>
+      </c>
+      <c r="D22">
+        <v>1438296</v>
+      </c>
+      <c r="E22">
+        <v>1247512</v>
+      </c>
+      <c r="F22">
+        <v>1438910</v>
+      </c>
+      <c r="G22">
+        <v>1230792</v>
+      </c>
+      <c r="H22">
+        <v>1438801</v>
+      </c>
+      <c r="I22">
+        <v>1233541</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23">
+        <v>1401147</v>
+      </c>
+      <c r="C23">
+        <v>40</v>
+      </c>
+      <c r="D23">
+        <v>107</v>
+      </c>
+      <c r="E23">
+        <v>265</v>
+      </c>
+      <c r="F23">
+        <v>544</v>
+      </c>
+      <c r="G23">
+        <v>1139</v>
+      </c>
+      <c r="H23">
+        <v>2445</v>
+      </c>
+      <c r="I23">
+        <v>5137</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24">
+        <v>1303082</v>
+      </c>
+      <c r="C24">
+        <v>1850386</v>
+      </c>
+      <c r="D24">
+        <v>1327536</v>
+      </c>
+      <c r="E24">
+        <v>824253</v>
+      </c>
+      <c r="F24">
+        <v>413418</v>
+      </c>
+      <c r="G24">
+        <v>245087</v>
+      </c>
+      <c r="H24">
+        <v>167994</v>
+      </c>
+      <c r="I24">
+        <v>51203</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25">
+        <v>1191029</v>
+      </c>
+      <c r="C25">
+        <v>1180264</v>
+      </c>
+      <c r="D25">
+        <v>1123372</v>
+      </c>
+      <c r="E25">
+        <v>1189681</v>
+      </c>
+      <c r="F25">
+        <v>1200067</v>
+      </c>
+      <c r="G25">
+        <v>1228259</v>
+      </c>
+      <c r="H25">
+        <v>1205112</v>
+      </c>
+      <c r="I25">
+        <v>1179244</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26">
+        <v>3421422</v>
+      </c>
+      <c r="C26">
+        <v>4856188</v>
+      </c>
+      <c r="D26">
+        <v>4855373</v>
+      </c>
+      <c r="E26">
+        <v>4557720</v>
+      </c>
+      <c r="F26">
+        <v>4723686</v>
+      </c>
+      <c r="G26">
+        <v>3093845</v>
+      </c>
+      <c r="H26">
+        <v>3169190</v>
+      </c>
+      <c r="I26">
+        <v>2640398</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27">
+        <v>2642745</v>
+      </c>
+      <c r="C27">
+        <v>2716931</v>
+      </c>
+      <c r="D27">
+        <v>3473391</v>
+      </c>
+      <c r="E27">
+        <v>2658225</v>
+      </c>
+      <c r="F27">
+        <v>2654354</v>
+      </c>
+      <c r="G27">
+        <v>3450999</v>
+      </c>
+      <c r="H27">
+        <v>2577043</v>
+      </c>
+      <c r="I27">
+        <v>2596864</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28">
+        <v>3960868</v>
+      </c>
+      <c r="C28">
+        <v>852</v>
+      </c>
+      <c r="D28">
+        <v>370</v>
+      </c>
+      <c r="E28">
+        <v>684</v>
+      </c>
+      <c r="F28">
+        <v>1696</v>
+      </c>
+      <c r="G28">
+        <v>6064</v>
+      </c>
+      <c r="H28">
+        <v>142</v>
+      </c>
+      <c r="I28">
+        <v>16590</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29">
+        <v>2581570</v>
+      </c>
+      <c r="C29">
+        <v>2590346</v>
+      </c>
+      <c r="D29">
+        <v>2504325</v>
+      </c>
+      <c r="E29">
+        <v>1355264</v>
+      </c>
+      <c r="F29">
+        <v>616020</v>
+      </c>
+      <c r="G29">
+        <v>252520</v>
+      </c>
+      <c r="H29">
+        <v>74205</v>
+      </c>
+      <c r="I29">
+        <v>29459</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30">
         <v>2560144</v>
       </c>
-      <c r="C22">
+      <c r="C30">
         <v>3529022</v>
       </c>
-      <c r="D22">
+      <c r="D30">
         <v>2567171</v>
       </c>
-      <c r="E22">
+      <c r="E30">
         <v>2586400</v>
       </c>
-      <c r="F22">
+      <c r="F30">
         <v>2599223</v>
       </c>
-      <c r="G22">
+      <c r="G30">
         <v>2575840</v>
       </c>
-      <c r="H22">
+      <c r="H30">
         <v>2522506</v>
       </c>
-      <c r="I22">
+      <c r="I30">
         <v>2445529</v>
       </c>
     </row>

</xml_diff>